<commit_message>
Added misc. electronic components
</commit_message>
<xml_diff>
--- a/Assembly/Volumetric peristaltic pump BOM.xlsx
+++ b/Assembly/Volumetric peristaltic pump BOM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tommystyrvoky/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tommystyrvoky/Documents/GitHub/Volumetric-peristaltic-pump-/Assembly/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{14817E47-4E13-074D-B2A9-3577B715098C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73026B54-C89E-9446-A84D-181E3A916253}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1360" yWindow="460" windowWidth="24240" windowHeight="13500" xr2:uid="{490480C7-9317-AB4D-B91B-DC41A9EB3E34}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="57">
   <si>
     <t>Part</t>
   </si>
@@ -190,6 +190,12 @@
   </si>
   <si>
     <t>cost each</t>
+  </si>
+  <si>
+    <t>1N4004 diode</t>
+  </si>
+  <si>
+    <t>200 Ω resistor</t>
   </si>
 </sst>
 </file>
@@ -612,7 +618,7 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+      <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1022,20 +1028,36 @@
         <v>30</v>
       </c>
     </row>
+    <row r="16" spans="1:8">
+      <c r="A16" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+    </row>
     <row r="17" spans="1:5">
-      <c r="A17" s="11" t="s">
+      <c r="A17" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="12">
+      <c r="B19" s="11"/>
+      <c r="C19" s="12">
         <f>SUM(C2:C15)</f>
         <v>167.48000000000002</v>
       </c>
-      <c r="D17" s="13">
+      <c r="D19" s="13">
         <f>SUM(D2:D10,D12:D14,13)</f>
         <v>68</v>
       </c>
-      <c r="E17" s="12">
+      <c r="E19" s="12">
         <f>SUM(E2:E15)</f>
         <v>100.78330000000001</v>
       </c>

</xml_diff>

<commit_message>
added print orientation photo
</commit_message>
<xml_diff>
--- a/Assembly/Volumetric peristaltic pump BOM.xlsx
+++ b/Assembly/Volumetric peristaltic pump BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tommystyrvoky/Documents/GitHub/Volumetric-peristaltic-pump-/Assembly/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73026B54-C89E-9446-A84D-181E3A916253}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E939A8FE-64AE-FE46-B9AE-ACB7AA3A59FE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1360" yWindow="460" windowWidth="24240" windowHeight="13500" xr2:uid="{490480C7-9317-AB4D-B91B-DC41A9EB3E34}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="58">
   <si>
     <t>Part</t>
   </si>
@@ -196,6 +196,9 @@
   </si>
   <si>
     <t>200 Ω resistor</t>
+  </si>
+  <si>
+    <t>Prefboard 61mm*61mm</t>
   </si>
 </sst>
 </file>
@@ -618,7 +621,7 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1041,6 +1044,14 @@
         <v>55</v>
       </c>
       <c r="D17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18">
         <v>1</v>
       </c>
     </row>

</xml_diff>